<commit_message>
Minor changes to Datasheets
</commit_message>
<xml_diff>
--- a/Element_Features_Data.xlsx
+++ b/Element_Features_Data.xlsx
@@ -1,26 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6th Semester Material\Project\Enhanced-Opposing-Properties-ML\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948DF501-4AEF-4347-9BB9-C76BBC00B869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -71,20 +60,19 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-3</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> kg)</t>
     </r>
@@ -95,39 +83,37 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>2</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> g</t>
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -138,39 +124,37 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>2</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> g</t>
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -181,39 +165,37 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>2</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> g</t>
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -224,39 +206,37 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>2</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> g</t>
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -282,20 +262,19 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -306,20 +285,19 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -330,20 +308,19 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -360,20 +337,19 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-1/3</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -390,20 +366,19 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -438,20 +413,19 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -462,20 +436,19 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -486,20 +459,19 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -510,20 +482,19 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -534,20 +505,19 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -558,20 +528,19 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -654,39 +623,37 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>-2</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> nm</t>
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>3</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -697,20 +664,19 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>2</t>
     </r>
     <r>
       <rPr>
         <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -734,8 +700,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -744,29 +711,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.5"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="7.5"/>
-      <color theme="1"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -777,7 +737,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -789,10 +749,10 @@
       <left/>
       <right/>
       <top style="thick">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -800,8 +760,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -810,7 +777,7 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -818,44 +785,62 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+  <cellXfs count="16">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -866,10 +851,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -896,82 +881,82 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -983,159 +968,189 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" customWidth="1"/>
+    <col min="1" max="1" style="13" width="47.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1154,1810 +1169,1808 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="5">
         <v>29</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>28</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="5">
         <v>30</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="5">
         <v>50</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="5">
         <v>82</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="5">
         <v>15</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>78</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <v>77</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="5">
         <v>79</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="5">
         <v>63</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="5">
         <v>45</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="5">
         <v>90</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="5">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="5">
         <v>26</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>27</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <v>25</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="5">
         <v>41</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="5">
         <v>59</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="5">
         <v>14</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="5">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="5">
         <v>75</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="5">
         <v>76</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="5">
         <v>74</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="5">
         <v>54</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="5">
         <v>22</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="5">
         <v>89</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="5">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="5">
         <v>4</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>4</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="5">
         <v>5</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>6</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="5">
         <v>3</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3">
-        <v>63.545999999999999</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B7" s="6">
+        <v>63.546</v>
+      </c>
+      <c r="C7" s="6">
         <v>58.69</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
         <v>65.39</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="6">
         <v>118.71</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="6">
         <v>207.2</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="6">
         <v>30.974</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="6">
         <v>24.305</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="6">
         <v>50.9</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="6">
         <v>46.6</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="6">
         <v>55.4</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="6">
         <v>31.1</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="5">
         <v>120</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="6">
         <v>7.89</v>
       </c>
-      <c r="H8" s="3">
-        <v>4.1100000000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="6">
+        <v>4.11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="5">
         <v>166</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="5">
         <v>144</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="5">
         <v>189</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="5">
         <v>662</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="5">
         <v>579</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="5">
         <v>229</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="5">
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="5">
         <v>53</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="6">
         <v>45.7</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="6">
         <v>60.3</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="5">
         <v>256</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="5">
         <v>232</v>
       </c>
-      <c r="G10" s="3">
-        <v>74.099999999999994</v>
-      </c>
-      <c r="H10" s="3">
+      <c r="G10" s="6">
+        <v>74.1</v>
+      </c>
+      <c r="H10" s="6">
         <v>38.6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="5">
         <v>103</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="6">
         <v>88.6</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="5">
         <v>117</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="5">
         <v>451</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="5">
         <v>402</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="5">
         <v>142</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="6">
         <v>74.8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="8">
         <v>1.45</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="8">
         <v>1.41</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="8">
         <v>1.49</v>
       </c>
-      <c r="E12" s="6">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="F12" s="6">
+      <c r="E12" s="8">
+        <v>2.24</v>
+      </c>
+      <c r="F12" s="8">
         <v>3.28</v>
       </c>
-      <c r="G12" s="3">
-        <v>0.34100000000000003</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.28799999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="6">
+        <v>0.341</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.288</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="6">
         <v>1.08</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="6">
         <v>1.76</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="6">
         <v>1.44</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="6">
         <v>1.88</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="6">
         <v>1.92</v>
       </c>
-      <c r="G13" s="3">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="G13" s="6">
+        <v>2.32</v>
+      </c>
+      <c r="H13" s="6">
         <v>1.31</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="6">
         <v>1.9</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="6">
         <v>1.9</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="6">
         <v>1.6</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="6">
         <v>1.8</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="6">
         <v>1.9</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="6">
         <v>2.1</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="6">
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="6">
         <v>1.75</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="6">
         <v>1.75</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="6">
         <v>1.66</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="6">
         <v>1.72</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="6">
         <v>1.55</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="6">
         <v>2.06</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="6">
         <v>1.23</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="3">
-        <v>4.4800000000000004</v>
-      </c>
-      <c r="C16" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D16" s="3">
+      <c r="B16" s="6">
+        <v>4.48</v>
+      </c>
+      <c r="C16" s="6">
+        <v>4.4</v>
+      </c>
+      <c r="D16" s="6">
         <v>4.45</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="6">
         <v>4.3</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="6">
         <v>3.9</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="6">
         <v>5.62</v>
       </c>
-      <c r="H16" s="3">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="6">
+        <v>8.3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="6">
         <v>745.4</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="6">
         <v>736.7</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="6">
         <v>906.4</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="6">
         <v>708.6</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="6">
         <v>715.5</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="6">
         <v>1011.7</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="6">
         <v>737.7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="5">
         <v>1958</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="5">
         <v>1753</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="5">
         <v>1733</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="5">
         <v>1412</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="5">
         <v>1450</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="5">
         <v>1903</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="5">
         <v>1451</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="5">
         <v>3554</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="5">
         <v>3393</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="5">
         <v>3833</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="5">
         <v>2943</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="5">
         <v>3081</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="5">
         <v>2912</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="5">
         <v>7733</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="6">
         <v>4.45</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="6">
         <v>5.2</v>
       </c>
-      <c r="D20" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E20" s="3">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="F20" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="G20" s="3">
+      <c r="D20" s="6">
+        <v>4.1</v>
+      </c>
+      <c r="E20" s="6">
+        <v>4.15</v>
+      </c>
+      <c r="F20" s="6">
+        <v>4.1</v>
+      </c>
+      <c r="G20" s="6">
         <v>5.55</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="6">
         <v>3.45</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="35.25">
       <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C21" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="D21" s="3">
+      <c r="B21" s="6">
+        <v>4.6</v>
+      </c>
+      <c r="C21" s="6">
+        <v>5.1</v>
+      </c>
+      <c r="D21" s="6">
         <v>4.2</v>
       </c>
-      <c r="E21" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="F21" s="3">
+      <c r="E21" s="6">
+        <v>4.4</v>
+      </c>
+      <c r="F21" s="5">
         <v>4</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="5">
         <v>0</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="6">
         <v>3.7</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="35.25">
       <c r="A22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="6">
         <v>1.47</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="6">
         <v>1.75</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="6">
         <v>1.32</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="6">
         <v>1.24</v>
       </c>
-      <c r="F22" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="F22" s="6">
+        <v>1.15</v>
+      </c>
+      <c r="G22" s="6">
         <v>1.65</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="6">
         <v>1.17</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="35.25">
       <c r="A23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="6">
         <v>4.2</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="6">
         <v>4.05</v>
       </c>
-      <c r="D23" s="3">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="E23" s="3">
+      <c r="D23" s="6">
+        <v>4.35</v>
+      </c>
+      <c r="E23" s="6">
         <v>5.65</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="6">
         <v>5.65</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="6">
         <v>4.8</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="6">
         <v>2.85</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="35.25">
       <c r="A24" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="6">
         <v>5.84</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="6">
         <v>5.71</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="6">
         <v>5.97</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="6">
         <v>9.1</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="6">
         <v>12.29</v>
       </c>
-      <c r="G24" s="3">
-        <v>4.8899999999999997</v>
-      </c>
-      <c r="H24" s="3">
+      <c r="G24" s="6">
+        <v>4.89</v>
+      </c>
+      <c r="H24" s="6">
         <v>3.31</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="35.25">
+      <c r="A25" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="8">
         <v>118.4</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="9">
         <v>112</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="9">
         <v>0</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="8">
         <v>107.3</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="8">
         <v>35.1</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="5">
         <v>72</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="35.25">
       <c r="A26" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="5">
         <v>11</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="5">
         <v>10</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="5">
         <v>12</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="5">
         <v>4</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="5">
         <v>4</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="5">
         <v>5</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="35.25">
       <c r="A27" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="5">
         <v>11</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="5">
         <v>10</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="5">
         <v>12</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="5">
         <v>4</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="5">
         <v>4</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="5">
         <v>5</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="35.25">
       <c r="A28" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="5">
         <v>1</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="5">
         <v>2</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="5">
         <v>2</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="5">
         <v>2</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="5">
         <v>2</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="5">
         <v>2</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="35.25">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="5">
         <v>0</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="5">
         <v>0</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="5">
         <v>0</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="5">
         <v>2</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="5">
         <v>2</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="5">
         <v>3</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="35.25">
       <c r="A30" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="5">
         <v>10</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="5">
         <v>8</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="5">
         <v>10</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="5">
         <v>0</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="5">
         <v>0</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="5">
         <v>0</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="35.25">
+      <c r="A31" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="9">
         <v>0</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="9">
         <v>0</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="9">
         <v>0</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="9">
         <v>0</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="9">
         <v>0</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="5">
         <v>0</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="35.25">
       <c r="A32" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="5">
         <v>1356</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="5">
         <v>1726</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="5">
         <v>693</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="5">
         <v>505</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="5">
         <v>601</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32" s="5">
         <v>317</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="5">
         <v>922</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="35.25">
       <c r="A33" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="5">
         <v>2840</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="5">
         <v>3005</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="5">
         <v>1180</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="5">
         <v>2543</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="5">
         <v>2013</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G33" s="5">
         <v>553</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="5">
         <v>1363</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="35.25">
       <c r="A34" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="6">
         <v>306.7</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="6">
         <v>374.8</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="6">
         <v>114.2</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="6">
         <v>296.2</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="6">
         <v>177.8</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="6">
         <v>51.9</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="6">
         <v>127.6</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="35.25">
       <c r="A35" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="5">
         <v>13</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="6">
         <v>17.2</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="6">
         <v>7.28</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="6">
         <v>7.07</v>
       </c>
-      <c r="F35" s="3">
-        <v>4.8099999999999996</v>
-      </c>
-      <c r="G35" s="3">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="H35" s="3">
+      <c r="F35" s="6">
+        <v>4.81</v>
+      </c>
+      <c r="G35" s="6">
+        <v>2.51</v>
+      </c>
+      <c r="H35" s="6">
         <v>8.9</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="35.25">
       <c r="A36" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="6">
         <v>338.3</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="6">
         <v>429.7</v>
       </c>
-      <c r="D36" s="3">
-        <v>130.69999999999999</v>
-      </c>
-      <c r="E36" s="3">
-        <v>302.10000000000002</v>
-      </c>
-      <c r="F36" s="3">
+      <c r="D36" s="6">
+        <v>130.7</v>
+      </c>
+      <c r="E36" s="6">
+        <v>302.1</v>
+      </c>
+      <c r="F36" s="5">
         <v>195</v>
       </c>
-      <c r="G36" s="3">
-        <v>314.60000000000002</v>
-      </c>
-      <c r="H36" s="3">
-        <v>147.69999999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G36" s="6">
+        <v>314.6</v>
+      </c>
+      <c r="H36" s="6">
+        <v>147.7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="35.25">
       <c r="A37" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="5">
         <v>95</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="5">
         <v>121</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="5">
         <v>61</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="5">
         <v>62</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="5">
         <v>57</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37" s="5">
         <v>62</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H37" s="5">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="35.25">
       <c r="A38" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="5">
         <v>100</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="5">
         <v>130</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="5">
         <v>50</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="5">
         <v>50</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="5">
         <v>48</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38" s="5">
         <v>50</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="35.25">
       <c r="A39" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="6">
         <v>3.49</v>
       </c>
-      <c r="C39" s="3">
-        <v>4.4400000000000004</v>
-      </c>
-      <c r="D39" s="3">
+      <c r="C39" s="6">
+        <v>4.44</v>
+      </c>
+      <c r="D39" s="6">
         <v>1.35</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="6">
         <v>3.14</v>
       </c>
-      <c r="F39" s="3">
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="G39" s="3">
+      <c r="F39" s="6">
+        <v>2.03</v>
+      </c>
+      <c r="G39" s="6">
         <v>3.43</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="6">
         <v>1.51</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="35.25">
       <c r="A40" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="6">
         <v>1.37</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="6">
         <v>1.86</v>
       </c>
-      <c r="D40" s="3">
-        <v>0.59799999999999998</v>
-      </c>
-      <c r="E40" s="3">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="F40" s="3">
+      <c r="D40" s="6">
+        <v>0.598</v>
+      </c>
+      <c r="E40" s="6">
+        <v>1.11</v>
+      </c>
+      <c r="F40" s="6">
         <v>0.43</v>
       </c>
-      <c r="G40" s="3">
-        <v>0.30399999999999999</v>
-      </c>
-      <c r="H40" s="3">
-        <v>0.35399999999999998</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G40" s="6">
+        <v>0.304</v>
+      </c>
+      <c r="H40" s="6">
+        <v>0.354</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="35.25">
       <c r="A41" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="3">
-        <v>137.80000000000001</v>
-      </c>
-      <c r="C41" s="3">
+      <c r="B41" s="6">
+        <v>137.8</v>
+      </c>
+      <c r="C41" s="6">
         <v>177.3</v>
       </c>
-      <c r="D41" s="3">
-        <v>69.400000000000006</v>
-      </c>
-      <c r="E41" s="3">
+      <c r="D41" s="6">
+        <v>69.4</v>
+      </c>
+      <c r="E41" s="6">
         <v>58.2</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="6">
         <v>45.8</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="5">
         <v>0</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="6">
         <v>35.6</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="35.25">
       <c r="A42" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="6">
         <v>48.4</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="5">
         <v>76</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="6">
         <v>41.9</v>
       </c>
-      <c r="E42" s="3">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="F42" s="3">
+      <c r="E42" s="6">
+        <v>18.4</v>
+      </c>
+      <c r="F42" s="6">
         <v>5.59</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="5">
         <v>0</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="6">
         <v>17.3</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="35.25">
+      <c r="A43" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="6">
-        <v>129.80000000000001</v>
-      </c>
-      <c r="C43" s="6">
+      <c r="B43" s="8">
+        <v>129.8</v>
+      </c>
+      <c r="C43" s="8">
         <v>199.5</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="8">
         <v>104.5</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="8">
         <v>49.9</v>
       </c>
-      <c r="F43" s="6">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="G43" s="3">
+      <c r="F43" s="8">
+        <v>16.1</v>
+      </c>
+      <c r="G43" s="5">
         <v>0</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="6">
         <v>44.7</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="35.25">
       <c r="A44" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="5">
         <v>66</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="5">
         <v>63</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="5">
         <v>69</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="5">
         <v>80</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="5">
         <v>81</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G44" s="5">
         <v>83</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="35.25">
       <c r="A45" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="5">
         <v>36</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="5">
         <v>39</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="5">
         <v>33</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="5">
         <v>26</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="5">
         <v>27</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G45" s="5">
         <v>19</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="5">
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="35.25">
       <c r="A46" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="5">
         <v>68</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="5">
         <v>65</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="5">
         <v>71</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="5">
         <v>78</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46" s="5">
         <v>77</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G46" s="5">
         <v>85</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="35.25">
       <c r="A47" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="5">
         <v>38</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="5">
         <v>41</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="5">
         <v>35</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="5">
         <v>24</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47" s="5">
         <v>23</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47" s="5">
         <v>21</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47" s="5">
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="35.25">
       <c r="A48" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="5">
         <v>72</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="5">
         <v>67</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="5">
         <v>76</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="5">
         <v>83</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F48" s="5">
         <v>82</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G48" s="5">
         <v>90</v>
       </c>
-      <c r="H48" s="3">
+      <c r="H48" s="5">
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="35.25">
       <c r="A49" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="5">
         <v>72</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="5">
         <v>69</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="5">
         <v>75</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="5">
         <v>82</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49" s="5">
         <v>81</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G49" s="5">
         <v>89</v>
       </c>
-      <c r="H49" s="3">
+      <c r="H49" s="5">
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="35.25">
       <c r="A50" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="5">
         <v>16</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="5">
         <v>74</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="5">
         <v>18</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="5">
         <v>81</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F50" s="5">
         <v>80</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G50" s="5">
         <v>95</v>
       </c>
-      <c r="H50" s="3">
+      <c r="H50" s="5">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="35.25">
       <c r="A51" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="5">
         <v>67</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="5">
         <v>64</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="5">
         <v>70</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="5">
         <v>81</v>
       </c>
-      <c r="F51" s="3">
+      <c r="F51" s="5">
         <v>82</v>
       </c>
-      <c r="G51" s="3">
+      <c r="G51" s="5">
         <v>84</v>
       </c>
-      <c r="H51" s="3">
+      <c r="H51" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="35.25">
       <c r="A52" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="5">
         <v>35</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="5">
         <v>38</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="5">
         <v>32</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="5">
         <v>25</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F52" s="5">
         <v>26</v>
       </c>
-      <c r="G52" s="3">
+      <c r="G52" s="5">
         <v>18</v>
       </c>
-      <c r="H52" s="3">
+      <c r="H52" s="5">
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="35.25">
       <c r="A53" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="5">
         <v>69</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="5">
         <v>66</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="5">
         <v>72</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="5">
         <v>79</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F53" s="5">
         <v>78</v>
       </c>
-      <c r="G53" s="3">
+      <c r="G53" s="5">
         <v>86</v>
       </c>
-      <c r="H53" s="3">
+      <c r="H53" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="35.25">
       <c r="A54" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="5">
         <v>37</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="5">
         <v>40</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="5">
         <v>34</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E54" s="5">
         <v>23</v>
       </c>
-      <c r="F54" s="3">
+      <c r="F54" s="5">
         <v>22</v>
       </c>
-      <c r="G54" s="3">
+      <c r="G54" s="5">
         <v>20</v>
       </c>
-      <c r="H54" s="3">
+      <c r="H54" s="5">
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="35.25">
       <c r="A55" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="5">
         <v>65</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="5">
         <v>59</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="5">
         <v>70</v>
       </c>
-      <c r="E55" s="3">
+      <c r="E55" s="5">
         <v>81</v>
       </c>
-      <c r="F55" s="3">
+      <c r="F55" s="5">
         <v>82</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G55" s="5">
         <v>84</v>
       </c>
-      <c r="H55" s="3">
+      <c r="H55" s="5">
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="35.25">
       <c r="A56" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="5">
         <v>64</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="5">
         <v>61</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="5">
         <v>69</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E56" s="5">
         <v>80</v>
       </c>
-      <c r="F56" s="3">
+      <c r="F56" s="5">
         <v>81</v>
       </c>
-      <c r="G56" s="3">
+      <c r="G56" s="5">
         <v>83</v>
       </c>
-      <c r="H56" s="3">
+      <c r="H56" s="5">
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="35.25">
+      <c r="A57" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="9">
         <v>64</v>
       </c>
-      <c r="C57" s="6">
+      <c r="C57" s="9">
         <v>59</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D57" s="9">
         <v>69</v>
       </c>
-      <c r="E57" s="6">
+      <c r="E57" s="9">
         <v>80</v>
       </c>
-      <c r="F57" s="6">
+      <c r="F57" s="9">
         <v>81</v>
       </c>
-      <c r="G57" s="3">
+      <c r="G57" s="5">
         <v>83</v>
       </c>
-      <c r="H57" s="3">
+      <c r="H57" s="5">
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="35.25">
       <c r="A58" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="6">
         <v>2.04</v>
       </c>
-      <c r="C58" s="3">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="D58" s="3">
+      <c r="C58" s="6">
+        <v>2.18</v>
+      </c>
+      <c r="D58" s="6">
         <v>1.88</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E58" s="6">
         <v>1.88</v>
       </c>
-      <c r="F58" s="3">
+      <c r="F58" s="6">
         <v>2.09</v>
       </c>
-      <c r="G58" s="3">
+      <c r="G58" s="6">
         <v>1.24</v>
       </c>
-      <c r="H58" s="3">
-        <v>2.0299999999999998</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H58" s="6">
+        <v>2.03</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="35.25">
       <c r="A59" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="6">
         <v>0.96</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C59" s="6">
         <v>0.59</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="6">
         <v>0.78</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E59" s="6">
         <v>0.65</v>
       </c>
-      <c r="F59" s="3">
+      <c r="F59" s="6">
         <v>0.83</v>
       </c>
-      <c r="G59" s="3">
+      <c r="G59" s="6">
         <v>0.36</v>
       </c>
-      <c r="H59" s="3">
+      <c r="H59" s="6">
         <v>0.63</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="35.25">
       <c r="A60" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B60" s="5">
         <v>117</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C60" s="5">
         <v>115</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="5">
         <v>125</v>
       </c>
-      <c r="E60" s="3">
+      <c r="E60" s="5">
         <v>140</v>
       </c>
-      <c r="F60" s="3">
+      <c r="F60" s="5">
         <v>154</v>
       </c>
-      <c r="G60" s="3">
+      <c r="G60" s="5">
         <v>110</v>
       </c>
-      <c r="H60" s="3">
+      <c r="H60" s="5">
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="35.25">
       <c r="A61" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B61" s="6">
         <v>1.278</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C61" s="6">
         <v>1.246</v>
       </c>
-      <c r="D61" s="3">
-        <v>1.3939999999999999</v>
-      </c>
-      <c r="E61" s="3">
+      <c r="D61" s="6">
+        <v>1.394</v>
+      </c>
+      <c r="E61" s="6">
         <v>1.623</v>
       </c>
-      <c r="F61" s="3">
+      <c r="F61" s="6">
         <v>1.75</v>
       </c>
-      <c r="G61" s="3">
+      <c r="G61" s="6">
         <v>1.28</v>
       </c>
-      <c r="H61" s="3">
-        <v>1.6020000000000001</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H61" s="6">
+        <v>1.602</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="35.25">
       <c r="A62" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="3">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="C62" s="3">
+      <c r="B62" s="6">
+        <v>2.55</v>
+      </c>
+      <c r="C62" s="6">
         <v>2.9</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D62" s="6">
         <v>2.21</v>
       </c>
-      <c r="E62" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F62" s="3">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G62" s="3">
+      <c r="E62" s="6">
+        <v>2.3</v>
+      </c>
+      <c r="F62" s="6">
+        <v>2.32</v>
+      </c>
+      <c r="G62" s="6">
         <v>1.54</v>
       </c>
-      <c r="H62" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H62" s="6">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="35.25">
       <c r="A63" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B63" s="3">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="C63" s="3">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="D63" s="3">
+      <c r="B63" s="6">
+        <v>1.12</v>
+      </c>
+      <c r="C63" s="6">
+        <v>1.13</v>
+      </c>
+      <c r="D63" s="6">
         <v>1.25</v>
       </c>
-      <c r="E63" s="3">
+      <c r="E63" s="6">
         <v>1.41</v>
       </c>
-      <c r="F63" s="3">
+      <c r="F63" s="6">
         <v>1.43</v>
       </c>
-      <c r="G63" s="3">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="H63" s="3">
-        <v>1.0900000000000001</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G63" s="6">
+        <v>1.09</v>
+      </c>
+      <c r="H63" s="6">
+        <v>1.09</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="35.25">
       <c r="A64" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B64" s="3">
+      <c r="B64" s="6">
         <v>1.181</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C64" s="6">
         <v>1.093</v>
       </c>
-      <c r="D64" s="3">
-        <v>1.5209999999999999</v>
-      </c>
-      <c r="E64" s="3">
-        <v>2.7050000000000001</v>
-      </c>
-      <c r="F64" s="3">
-        <v>3.0339999999999998</v>
-      </c>
-      <c r="G64" s="3">
+      <c r="D64" s="6">
+        <v>1.521</v>
+      </c>
+      <c r="E64" s="6">
+        <v>2.705</v>
+      </c>
+      <c r="F64" s="6">
+        <v>3.034</v>
+      </c>
+      <c r="G64" s="6">
         <v>1.899</v>
       </c>
-      <c r="H64" s="3">
-        <v>2.3239999999999998</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H64" s="6">
+        <v>2.324</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="35.25">
       <c r="A65" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B65" s="6">
         <v>3.7</v>
       </c>
-      <c r="C65" s="3">
+      <c r="C65" s="6">
         <v>3.52</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D65" s="6">
         <v>4.38</v>
       </c>
-      <c r="E65" s="3">
+      <c r="E65" s="6">
         <v>6.43</v>
       </c>
-      <c r="F65" s="3">
+      <c r="F65" s="6">
         <v>6.94</v>
       </c>
-      <c r="G65" s="3">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="H65" s="3">
+      <c r="G65" s="6">
+        <v>4.15</v>
+      </c>
+      <c r="H65" s="6">
         <v>5.81</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="35.25">
       <c r="A66" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B66" s="5">
         <v>12</v>
       </c>
-      <c r="C66" s="3">
+      <c r="C66" s="5">
         <v>12</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D66" s="5">
         <v>12</v>
       </c>
-      <c r="E66" s="3">
+      <c r="E66" s="5">
         <v>3</v>
       </c>
-      <c r="F66" s="3">
+      <c r="F66" s="5">
         <v>12</v>
       </c>
-      <c r="G66" s="3">
+      <c r="G66" s="5">
         <v>3</v>
       </c>
-      <c r="H66" s="3">
+      <c r="H66" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="35.25">
       <c r="A67" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B67" s="6">
         <v>127.8</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C67" s="6">
         <v>124.6</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D67" s="6">
         <v>139.5</v>
       </c>
-      <c r="E67" s="3">
+      <c r="E67" s="5">
         <v>162</v>
       </c>
-      <c r="F67" s="3">
+      <c r="F67" s="5">
         <v>175</v>
       </c>
-      <c r="G67" s="3">
+      <c r="G67" s="5">
         <v>106</v>
       </c>
-      <c r="H67" s="3">
+      <c r="H67" s="6">
         <v>160.1</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="35.25">
       <c r="A68" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="6">
         <v>361.49</v>
       </c>
-      <c r="C68" s="3">
+      <c r="C68" s="6">
         <v>352.4</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D68" s="6">
         <v>266.49</v>
       </c>
-      <c r="E68" s="3">
-        <v>583.17999999999995</v>
-      </c>
-      <c r="F68" s="3">
+      <c r="E68" s="6">
+        <v>583.18</v>
+      </c>
+      <c r="F68" s="6">
         <v>495.08</v>
       </c>
-      <c r="G68" s="3">
-        <v>550.29999999999995</v>
-      </c>
-      <c r="H68" s="3">
+      <c r="G68" s="6">
+        <v>550.3</v>
+      </c>
+      <c r="H68" s="6">
         <v>320.94</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="35.25">
       <c r="A69" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B69" s="6">
         <v>361.49</v>
       </c>
-      <c r="C69" s="3">
+      <c r="C69" s="6">
         <v>352.4</v>
       </c>
-      <c r="D69" s="3">
+      <c r="D69" s="6">
         <v>266.49</v>
       </c>
-      <c r="E69" s="3">
-        <v>583.17999999999995</v>
-      </c>
-      <c r="F69" s="3">
+      <c r="E69" s="6">
+        <v>583.18</v>
+      </c>
+      <c r="F69" s="6">
         <v>495.08</v>
       </c>
-      <c r="G69" s="3">
-        <v>1126.0999999999999</v>
-      </c>
-      <c r="H69" s="3">
-        <v>521.08000000000004</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="7" t="s">
+      <c r="G69" s="6">
+        <v>1126.1</v>
+      </c>
+      <c r="H69" s="6">
+        <v>521.08</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="35.25">
+      <c r="A70" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="8">
+      <c r="B70" s="11">
         <v>361.49</v>
       </c>
-      <c r="C70" s="8">
+      <c r="C70" s="11">
         <v>352.4</v>
       </c>
-      <c r="D70" s="8">
+      <c r="D70" s="11">
         <v>494.68</v>
       </c>
-      <c r="E70" s="8">
+      <c r="E70" s="11">
         <v>318.19</v>
       </c>
-      <c r="F70" s="8">
+      <c r="F70" s="11">
         <v>495.08</v>
       </c>
-      <c r="G70" s="8">
+      <c r="G70" s="12">
         <v>106</v>
       </c>
-      <c r="H70" s="8">
+      <c r="H70" s="11">
         <v>160.1</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>